<commit_message>
Project layer sql server c#
Simple design connection in SQL Server database , to select and insert
records.
</commit_message>
<xml_diff>
--- a/HoursWork/Work-Hours/planilha/Planilha_Horas_02-2016.xlsx
+++ b/HoursWork/Work-Hours/planilha/Planilha_Horas_02-2016.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr showInkAnnotation="0" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costasa\Documents\GitHub\ASP.NET\HoursWork\Work-Hours\planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanta\Documents\GitHub\ASP.NET\HoursWork\Work-Hours\planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="02-2016" sheetId="1" r:id="rId1"/>
+    <sheet name="05-2016" sheetId="1" r:id="rId1"/>
     <sheet name="Consolidado" sheetId="9" state="hidden" r:id="rId2"/>
     <sheet name="Projetos" sheetId="10" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'02-2016'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'05-2016'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Projetos!$A$16:$B$80</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="0">'02-2016'!#REF!</definedName>
-    <definedName name="Front">'02-2016'!A1:A43</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">'05-2016'!#REF!</definedName>
+    <definedName name="Front">'05-2016'!A1:A43</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="349">
   <si>
     <t>Perfil do Profissional</t>
   </si>
@@ -1076,12 +1076,51 @@
   </si>
   <si>
     <t>HP</t>
+  </si>
+  <si>
+    <t>FERIAS</t>
+  </si>
+  <si>
+    <t>CARDS</t>
+  </si>
+  <si>
+    <t>GP For Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aguardando demanda </t>
+  </si>
+  <si>
+    <t>configuração do ambiente</t>
+  </si>
+  <si>
+    <t>desenvolvimento relatório x ajuste</t>
+  </si>
+  <si>
+    <t>entrega relatório x ajuste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aguardando retorno do cliente </t>
+  </si>
+  <si>
+    <t>alterações solicitado pelo cliente</t>
+  </si>
+  <si>
+    <t>aguardando Renato</t>
+  </si>
+  <si>
+    <t>FERIADO</t>
+  </si>
+  <si>
+    <t>entrega de pacote para produção</t>
+  </si>
+  <si>
+    <t>criação de documento para entedimento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="dddd"/>
@@ -1377,7 +1416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1921,6 +1960,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1948,7 +2040,7 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
@@ -2158,6 +2250,57 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="14" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="14" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="14" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="14" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2209,59 +2352,48 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="14" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="14" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="14" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="14" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
@@ -2290,7 +2422,103 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Sheet Title" xfId="23"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2373,30 +2601,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2413,7 +2617,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="eloi.takeuchi" refreshedDate="40469.379658449077" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="49">
   <cacheSource type="worksheet">
-    <worksheetSource ref="N10:P46" sheet="02-2016"/>
+    <worksheetSource ref="N10:P47" sheet="05-2016"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Front" numFmtId="0">
@@ -3524,11 +3728,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Lista1" displayName="Lista1" ref="A16:B80" insertRowShift="1" totalsRowShown="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Lista1" displayName="Lista1" ref="A16:B80" insertRowShift="1" totalsRowShown="0" headerRowBorderDxfId="18">
   <autoFilter ref="A16:B80"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Projetos_x000a_(SSEDS)" dataDxfId="1"/>
-    <tableColumn id="2" name="Descrição" dataDxfId="0"/>
+    <tableColumn id="1" name="Projetos_x000a_(SSEDS)" dataDxfId="17"/>
+    <tableColumn id="2" name="Descrição" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3610,6 +3814,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3645,6 +3866,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3824,13 +4062,13 @@
   <sheetPr codeName="Plan1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X67"/>
+  <dimension ref="A1:X68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomRight" activeCell="L26" sqref="L26:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3860,17 +4098,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="96"/>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
+      <c r="A1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
       <c r="L1" s="71"/>
       <c r="M1" s="28"/>
       <c r="N1"/>
@@ -3929,13 +4167,13 @@
       <c r="E4" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="F4" s="98"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="100"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="117"/>
       <c r="N4"/>
       <c r="O4"/>
       <c r="P4"/>
@@ -3952,15 +4190,15 @@
       <c r="E5" s="47" t="s">
         <v>334</v>
       </c>
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="118" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="103"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="120"/>
       <c r="M5" s="28"/>
       <c r="N5"/>
       <c r="O5"/>
@@ -3978,16 +4216,16 @@
       <c r="E6" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="F6" s="104">
-        <f>K41</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="103"/>
+      <c r="F6" s="121">
+        <f>K42</f>
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="120"/>
       <c r="M6" s="28"/>
       <c r="N6"/>
       <c r="O6"/>
@@ -4003,13 +4241,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="49"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="110"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="127"/>
       <c r="N7"/>
       <c r="O7"/>
       <c r="P7"/>
@@ -4024,7 +4262,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="84">
-        <v>42401</v>
+        <v>42491</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="35"/>
@@ -4040,30 +4278,30 @@
       <c r="R8"/>
     </row>
     <row r="9" spans="1:22" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="113" t="s">
+      <c r="D9" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="107" t="s">
+      <c r="E9" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="118"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="122" t="s">
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="103" t="s">
         <v>8</v>
       </c>
       <c r="Q9" s="2" t="str">
@@ -4076,11 +4314,11 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="106"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="107"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="124"/>
       <c r="F10" s="93" t="s">
         <v>9</v>
       </c>
@@ -4099,7 +4337,7 @@
       <c r="K10" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="122"/>
+      <c r="L10" s="103"/>
       <c r="N10" s="3" t="s">
         <v>15</v>
       </c>
@@ -4120,21 +4358,23 @@
     </row>
     <row r="11" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="94">
-        <v>42401</v>
+        <v>42491</v>
       </c>
       <c r="B11" s="63">
         <f t="shared" ref="B11:B15" si="0">A11</f>
-        <v>42401</v>
-      </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
+        <v>42491</v>
+      </c>
+      <c r="C11" s="134" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="135"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="135"/>
+      <c r="K11" s="136"/>
       <c r="L11" s="90">
         <f t="shared" ref="L11:L40" si="1">(G11-F11)+(I11-H11)+(K11-J11)</f>
         <v>0</v>
@@ -4161,21 +4401,21 @@
     <row r="12" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="94">
         <f t="shared" ref="A12:A16" si="2">A11+1</f>
-        <v>42402</v>
+        <v>42492</v>
       </c>
       <c r="B12" s="63">
         <f t="shared" si="0"/>
-        <v>42402</v>
-      </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
+        <v>42492</v>
+      </c>
+      <c r="C12" s="137"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="138"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="139"/>
       <c r="L12" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4202,21 +4442,21 @@
     <row r="13" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="94">
         <f t="shared" si="2"/>
-        <v>42403</v>
+        <v>42493</v>
       </c>
       <c r="B13" s="63">
         <f t="shared" ref="B13" si="3">A13</f>
-        <v>42403</v>
-      </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
+        <v>42493</v>
+      </c>
+      <c r="C13" s="137"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="139"/>
       <c r="L13" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4243,21 +4483,21 @@
     <row r="14" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="94">
         <f t="shared" si="2"/>
-        <v>42404</v>
+        <v>42494</v>
       </c>
       <c r="B14" s="63">
         <f t="shared" si="0"/>
-        <v>42404</v>
-      </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
+        <v>42494</v>
+      </c>
+      <c r="C14" s="137"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="138"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="139"/>
       <c r="L14" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4282,21 +4522,21 @@
     <row r="15" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="94">
         <f>A14+1</f>
-        <v>42405</v>
+        <v>42495</v>
       </c>
       <c r="B15" s="63">
         <f t="shared" si="0"/>
-        <v>42405</v>
-      </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
+        <v>42495</v>
+      </c>
+      <c r="C15" s="137"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
+      <c r="F15" s="138"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="139"/>
       <c r="L15" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4323,21 +4563,21 @@
     <row r="16" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="94">
         <f t="shared" si="2"/>
-        <v>42406</v>
+        <v>42496</v>
       </c>
       <c r="B16" s="63">
         <f t="shared" ref="B16" si="4">A16</f>
-        <v>42406</v>
-      </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86"/>
+        <v>42496</v>
+      </c>
+      <c r="C16" s="137"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="139"/>
       <c r="L16" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4365,21 +4605,21 @@
     <row r="17" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="94">
         <f>A16+1</f>
-        <v>42407</v>
+        <v>42497</v>
       </c>
       <c r="B17" s="63">
         <f t="shared" ref="B17:B39" si="5">A17</f>
-        <v>42407</v>
-      </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
+        <v>42497</v>
+      </c>
+      <c r="C17" s="137"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="138"/>
+      <c r="K17" s="139"/>
       <c r="L17" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4405,22 +4645,22 @@
     </row>
     <row r="18" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="94">
-        <f t="shared" ref="A18:A40" si="6">A17+1</f>
-        <v>42408</v>
+        <f t="shared" ref="A18:A41" si="6">A17+1</f>
+        <v>42498</v>
       </c>
       <c r="B18" s="63">
         <f t="shared" si="5"/>
-        <v>42408</v>
-      </c>
-      <c r="C18" s="95"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
+        <v>42498</v>
+      </c>
+      <c r="C18" s="140"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="141"/>
+      <c r="J18" s="141"/>
+      <c r="K18" s="142"/>
       <c r="L18" s="90">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4436,24 +4676,38 @@
     <row r="19" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="94">
         <f t="shared" si="6"/>
-        <v>42409</v>
+        <v>42499</v>
       </c>
       <c r="B19" s="63">
         <f t="shared" si="5"/>
-        <v>42409</v>
-      </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
+        <v>42499</v>
+      </c>
+      <c r="C19" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D19" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E19" s="133" t="s">
+        <v>339</v>
+      </c>
+      <c r="F19" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G19" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H19" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I19" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J19" s="86"/>
       <c r="K19" s="86"/>
       <c r="L19" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M19" s="80"/>
       <c r="N19" s="76"/>
@@ -4465,24 +4719,38 @@
     <row r="20" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="94">
         <f t="shared" si="6"/>
-        <v>42410</v>
+        <v>42500</v>
       </c>
       <c r="B20" s="63">
         <f t="shared" si="5"/>
-        <v>42410</v>
-      </c>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
+        <v>42500</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D20" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E20" s="133" t="s">
+        <v>340</v>
+      </c>
+      <c r="F20" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G20" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I20" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J20" s="86"/>
       <c r="K20" s="86"/>
       <c r="L20" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M20" s="80"/>
       <c r="N20" s="76"/>
@@ -4494,24 +4762,38 @@
     <row r="21" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="94">
         <f t="shared" si="6"/>
-        <v>42411</v>
+        <v>42501</v>
       </c>
       <c r="B21" s="63">
         <f t="shared" si="5"/>
-        <v>42411</v>
-      </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
+        <v>42501</v>
+      </c>
+      <c r="C21" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D21" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21" s="133" t="s">
+        <v>341</v>
+      </c>
+      <c r="F21" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G21" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I21" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J21" s="86"/>
       <c r="K21" s="86"/>
       <c r="L21" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M21" s="80"/>
       <c r="N21" s="76"/>
@@ -4523,24 +4805,38 @@
     <row r="22" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="94">
         <f t="shared" si="6"/>
-        <v>42412</v>
+        <v>42502</v>
       </c>
       <c r="B22" s="63">
         <f t="shared" si="5"/>
-        <v>42412</v>
-      </c>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
+        <v>42502</v>
+      </c>
+      <c r="C22" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D22" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E22" s="133" t="s">
+        <v>341</v>
+      </c>
+      <c r="F22" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G22" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I22" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J22" s="86"/>
       <c r="K22" s="86"/>
       <c r="L22" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M22" s="80"/>
       <c r="N22" s="76"/>
@@ -4554,24 +4850,38 @@
     <row r="23" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="94">
         <f t="shared" si="6"/>
-        <v>42413</v>
+        <v>42503</v>
       </c>
       <c r="B23" s="63">
         <f t="shared" si="5"/>
-        <v>42413</v>
-      </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
+        <v>42503</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="133" t="s">
+        <v>342</v>
+      </c>
+      <c r="F23" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G23" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I23" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J23" s="86"/>
       <c r="K23" s="86"/>
       <c r="L23" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M23" s="80"/>
       <c r="N23" s="76"/>
@@ -4583,11 +4893,11 @@
     <row r="24" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="94">
         <f t="shared" si="6"/>
-        <v>42414</v>
+        <v>42504</v>
       </c>
       <c r="B24" s="63">
         <f t="shared" si="5"/>
-        <v>42414</v>
+        <v>42504</v>
       </c>
       <c r="C24" s="95"/>
       <c r="D24" s="95"/>
@@ -4613,11 +4923,11 @@
     <row r="25" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="94">
         <f t="shared" si="6"/>
-        <v>42415</v>
+        <v>42505</v>
       </c>
       <c r="B25" s="63">
         <f t="shared" si="5"/>
-        <v>42415</v>
+        <v>42505</v>
       </c>
       <c r="C25" s="95"/>
       <c r="D25" s="95"/>
@@ -4642,24 +4952,38 @@
     <row r="26" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
         <f t="shared" si="6"/>
-        <v>42416</v>
+        <v>42506</v>
       </c>
       <c r="B26" s="63">
         <f t="shared" si="5"/>
-        <v>42416</v>
-      </c>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
+        <v>42506</v>
+      </c>
+      <c r="C26" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D26" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E26" s="133" t="s">
+        <v>343</v>
+      </c>
+      <c r="F26" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G26" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I26" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J26" s="86"/>
       <c r="K26" s="86"/>
       <c r="L26" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M26" s="80"/>
       <c r="N26" s="76"/>
@@ -4671,24 +4995,38 @@
     <row r="27" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="94">
         <f t="shared" si="6"/>
-        <v>42417</v>
+        <v>42507</v>
       </c>
       <c r="B27" s="63">
         <f t="shared" si="5"/>
-        <v>42417</v>
-      </c>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
+        <v>42507</v>
+      </c>
+      <c r="C27" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D27" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E27" s="133" t="s">
+        <v>344</v>
+      </c>
+      <c r="F27" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G27" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I27" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J27" s="86"/>
       <c r="K27" s="86"/>
       <c r="L27" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M27" s="80"/>
       <c r="N27" s="76"/>
@@ -4700,24 +5038,38 @@
     <row r="28" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="94">
         <f t="shared" si="6"/>
-        <v>42418</v>
+        <v>42508</v>
       </c>
       <c r="B28" s="63">
         <f t="shared" si="5"/>
-        <v>42418</v>
-      </c>
-      <c r="C28" s="95"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
+        <v>42508</v>
+      </c>
+      <c r="C28" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D28" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E28" s="133" t="s">
+        <v>344</v>
+      </c>
+      <c r="F28" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G28" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H28" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I28" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J28" s="86"/>
       <c r="K28" s="86"/>
       <c r="L28" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M28" s="80"/>
       <c r="N28" s="76"/>
@@ -4729,24 +5081,38 @@
     <row r="29" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="94">
         <f t="shared" si="6"/>
-        <v>42419</v>
+        <v>42509</v>
       </c>
       <c r="B29" s="63">
         <f t="shared" si="5"/>
-        <v>42419</v>
-      </c>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
-      <c r="H29" s="86"/>
-      <c r="I29" s="86"/>
+        <v>42509</v>
+      </c>
+      <c r="C29" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E29" s="133" t="s">
+        <v>345</v>
+      </c>
+      <c r="F29" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G29" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I29" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J29" s="91"/>
       <c r="K29" s="91"/>
       <c r="L29" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M29" s="80"/>
       <c r="N29" s="76"/>
@@ -4759,24 +5125,38 @@
     <row r="30" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="94">
         <f t="shared" si="6"/>
-        <v>42420</v>
+        <v>42510</v>
       </c>
       <c r="B30" s="63">
         <f t="shared" si="5"/>
-        <v>42420</v>
-      </c>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="86"/>
-      <c r="H30" s="86"/>
-      <c r="I30" s="86"/>
+        <v>42510</v>
+      </c>
+      <c r="C30" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D30" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E30" s="133" t="s">
+        <v>343</v>
+      </c>
+      <c r="F30" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G30" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I30" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J30" s="86"/>
       <c r="K30" s="86"/>
       <c r="L30" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M30" s="80"/>
       <c r="N30" s="76"/>
@@ -4788,15 +5168,15 @@
     <row r="31" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="94">
         <f t="shared" si="6"/>
-        <v>42421</v>
+        <v>42511</v>
       </c>
       <c r="B31" s="63">
         <f t="shared" si="5"/>
-        <v>42421</v>
+        <v>42511</v>
       </c>
       <c r="C31" s="95"/>
       <c r="D31" s="95"/>
-      <c r="E31" s="89"/>
+      <c r="E31" s="133"/>
       <c r="F31" s="86"/>
       <c r="G31" s="86"/>
       <c r="H31" s="86"/>
@@ -4817,15 +5197,15 @@
     <row r="32" spans="1:22" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="94">
         <f t="shared" si="6"/>
-        <v>42422</v>
+        <v>42512</v>
       </c>
       <c r="B32" s="63">
         <f t="shared" si="5"/>
-        <v>42422</v>
+        <v>42512</v>
       </c>
       <c r="C32" s="95"/>
       <c r="D32" s="95"/>
-      <c r="E32" s="89"/>
+      <c r="E32" s="133"/>
       <c r="F32" s="86"/>
       <c r="G32" s="86"/>
       <c r="H32" s="86"/>
@@ -4847,24 +5227,38 @@
     <row r="33" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="94">
         <f t="shared" si="6"/>
-        <v>42423</v>
+        <v>42513</v>
       </c>
       <c r="B33" s="63">
         <f t="shared" si="5"/>
-        <v>42423</v>
-      </c>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="86"/>
-      <c r="H33" s="86"/>
-      <c r="I33" s="86"/>
+        <v>42513</v>
+      </c>
+      <c r="C33" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D33" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E33" s="133" t="s">
+        <v>347</v>
+      </c>
+      <c r="F33" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G33" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I33" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J33" s="86"/>
       <c r="K33" s="86"/>
       <c r="L33" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M33" s="80"/>
       <c r="N33" s="76"/>
@@ -4876,24 +5270,38 @@
     <row r="34" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="94">
         <f t="shared" si="6"/>
-        <v>42424</v>
+        <v>42514</v>
       </c>
       <c r="B34" s="63">
         <f t="shared" si="5"/>
-        <v>42424</v>
-      </c>
-      <c r="C34" s="95"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
+        <v>42514</v>
+      </c>
+      <c r="C34" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D34" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E34" s="133" t="s">
+        <v>348</v>
+      </c>
+      <c r="F34" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G34" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H34" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I34" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J34" s="86"/>
       <c r="K34" s="86"/>
       <c r="L34" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M34" s="80"/>
       <c r="N34" s="76"/>
@@ -4905,24 +5313,38 @@
     <row r="35" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="94">
         <f t="shared" si="6"/>
-        <v>42425</v>
+        <v>42515</v>
       </c>
       <c r="B35" s="63">
         <f t="shared" si="5"/>
-        <v>42425</v>
-      </c>
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
+        <v>42515</v>
+      </c>
+      <c r="C35" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D35" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E35" s="133" t="s">
+        <v>348</v>
+      </c>
+      <c r="F35" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G35" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H35" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I35" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J35" s="86"/>
       <c r="K35" s="86"/>
       <c r="L35" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M35" s="80"/>
       <c r="N35" s="76"/>
@@ -4935,15 +5357,17 @@
     <row r="36" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="94">
         <f t="shared" si="6"/>
-        <v>42426</v>
+        <v>42516</v>
       </c>
       <c r="B36" s="63">
         <f t="shared" si="5"/>
-        <v>42426</v>
-      </c>
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="89"/>
+        <v>42516</v>
+      </c>
+      <c r="C36" s="143" t="s">
+        <v>346</v>
+      </c>
+      <c r="D36" s="144"/>
+      <c r="E36" s="145"/>
       <c r="F36" s="86"/>
       <c r="G36" s="86"/>
       <c r="H36" s="86"/>
@@ -4966,24 +5390,38 @@
     <row r="37" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="94">
         <f t="shared" si="6"/>
-        <v>42427</v>
+        <v>42517</v>
       </c>
       <c r="B37" s="63">
         <f t="shared" si="5"/>
-        <v>42427</v>
-      </c>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
+        <v>42517</v>
+      </c>
+      <c r="C37" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D37" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E37" s="133" t="s">
+        <v>348</v>
+      </c>
+      <c r="F37" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G37" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H37" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I37" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J37" s="86"/>
       <c r="K37" s="86"/>
       <c r="L37" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M37" s="80"/>
       <c r="N37" s="76"/>
@@ -4995,11 +5433,11 @@
     <row r="38" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="94">
         <f t="shared" si="6"/>
-        <v>42428</v>
+        <v>42518</v>
       </c>
       <c r="B38" s="63">
         <f t="shared" si="5"/>
-        <v>42428</v>
+        <v>42518</v>
       </c>
       <c r="C38" s="95"/>
       <c r="D38" s="95"/>
@@ -5024,11 +5462,11 @@
     <row r="39" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="94">
         <f t="shared" si="6"/>
-        <v>42429</v>
+        <v>42519</v>
       </c>
       <c r="B39" s="63">
         <f t="shared" si="5"/>
-        <v>42429</v>
+        <v>42519</v>
       </c>
       <c r="C39" s="95"/>
       <c r="D39" s="95"/>
@@ -5053,24 +5491,38 @@
     <row r="40" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="94">
         <f t="shared" si="6"/>
-        <v>42430</v>
+        <v>42520</v>
       </c>
       <c r="B40" s="95">
         <f t="shared" ref="B40" si="7">A40</f>
-        <v>42430</v>
-      </c>
-      <c r="C40" s="95"/>
-      <c r="D40" s="95"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
+        <v>42520</v>
+      </c>
+      <c r="C40" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D40" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E40" s="133" t="s">
+        <v>339</v>
+      </c>
+      <c r="F40" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G40" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H40" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I40" s="86">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J40" s="86"/>
       <c r="K40" s="86"/>
       <c r="L40" s="90">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M40" s="80"/>
       <c r="N40" s="76"/>
@@ -5079,492 +5531,535 @@
       <c r="Q40" s="79"/>
       <c r="R40" s="79"/>
     </row>
-    <row r="41" spans="1:24" s="37" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="127" t="s">
+    <row r="41" spans="1:24" s="75" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="94">
+        <f t="shared" si="6"/>
+        <v>42521</v>
+      </c>
+      <c r="B41" s="95">
+        <f t="shared" ref="B41" si="8">A41</f>
+        <v>42521</v>
+      </c>
+      <c r="C41" s="95" t="s">
+        <v>337</v>
+      </c>
+      <c r="D41" s="95" t="s">
+        <v>338</v>
+      </c>
+      <c r="E41" s="133" t="s">
+        <v>339</v>
+      </c>
+      <c r="F41" s="86">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G41" s="86">
+        <v>0.5</v>
+      </c>
+      <c r="H41" s="86">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I41" s="86">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="J41" s="86"/>
+      <c r="K41" s="86"/>
+      <c r="L41" s="90">
+        <f t="shared" ref="L41" si="9">(G41-F41)+(I41-H41)+(K41-J41)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M41" s="80"/>
+      <c r="N41" s="76"/>
+      <c r="O41" s="77"/>
+      <c r="P41" s="78"/>
+      <c r="Q41" s="79"/>
+      <c r="R41" s="79"/>
+    </row>
+    <row r="42" spans="1:24" s="37" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="128"/>
-      <c r="C41" s="128"/>
-      <c r="D41" s="128"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="128"/>
-      <c r="G41" s="128"/>
-      <c r="H41" s="128"/>
-      <c r="I41" s="128"/>
-      <c r="J41" s="129"/>
-      <c r="K41" s="130">
+      <c r="B42" s="109"/>
+      <c r="C42" s="109"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="109"/>
+      <c r="F42" s="109"/>
+      <c r="G42" s="109"/>
+      <c r="H42" s="109"/>
+      <c r="I42" s="109"/>
+      <c r="J42" s="110"/>
+      <c r="K42" s="111">
         <f>SUM(L11:L40)</f>
-        <v>0</v>
-      </c>
-      <c r="L41" s="131"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="3" t="s">
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="L42" s="112"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="O41" s="13" t="s">
+      <c r="O42" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="P41" s="11" t="s">
+      <c r="P42" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="2" t="str">
+      <c r="Q42" s="1"/>
+      <c r="R42" s="2" t="str">
         <f>IF(Projetos!A71&gt;0,Projetos!A71,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="123"/>
-      <c r="B42" s="123"/>
-      <c r="C42" s="123"/>
-      <c r="D42" s="123"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="125"/>
-      <c r="G42" s="125"/>
-      <c r="H42" s="125"/>
-      <c r="I42" s="125"/>
-      <c r="J42" s="125"/>
-      <c r="K42" s="125"/>
-      <c r="L42" s="125"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="3" t="s">
+    <row r="43" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="104"/>
+      <c r="B43" s="104"/>
+      <c r="C43" s="104"/>
+      <c r="D43" s="104"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="106"/>
+      <c r="G43" s="106"/>
+      <c r="H43" s="106"/>
+      <c r="I43" s="106"/>
+      <c r="J43" s="106"/>
+      <c r="K43" s="106"/>
+      <c r="L43" s="106"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="O42" s="13" t="s">
+      <c r="O43" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="P42" s="11" t="s">
+      <c r="P43" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="2" t="str">
+      <c r="Q43" s="12"/>
+      <c r="R43" s="2" t="str">
         <f>IF(Projetos!A72&gt;0,Projetos!A72,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="124"/>
-      <c r="B43" s="124"/>
-      <c r="C43" s="124"/>
-      <c r="D43" s="124"/>
-      <c r="E43" s="124"/>
-      <c r="F43" s="126"/>
-      <c r="G43" s="126"/>
-      <c r="H43" s="126"/>
-      <c r="I43" s="126"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="126"/>
-      <c r="L43" s="126"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="3" t="s">
+    <row r="44" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="105"/>
+      <c r="B44" s="105"/>
+      <c r="C44" s="105"/>
+      <c r="D44" s="105"/>
+      <c r="E44" s="105"/>
+      <c r="F44" s="107"/>
+      <c r="G44" s="107"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="107"/>
+      <c r="K44" s="107"/>
+      <c r="L44" s="107"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="O43" s="13" t="s">
+      <c r="O44" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="P43" s="11" t="s">
+      <c r="P44" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="2" t="str">
+      <c r="Q44" s="12"/>
+      <c r="R44" s="2" t="str">
         <f>IF(Projetos!A73&gt;0,Projetos!A73,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="115" t="s">
+    <row r="45" spans="1:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="115"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="115"/>
-      <c r="F44" s="116" t="s">
+      <c r="B45" s="96"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="116"/>
-      <c r="H44" s="116"/>
-      <c r="I44" s="116"/>
-      <c r="J44" s="116"/>
-      <c r="K44" s="116"/>
-      <c r="L44" s="116"/>
-      <c r="N44" s="3" t="s">
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="97"/>
+      <c r="K45" s="97"/>
+      <c r="L45" s="97"/>
+      <c r="N45" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="O44" s="13" t="s">
+      <c r="O45" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="P44" s="4" t="s">
+      <c r="P45" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="R44" s="2" t="str">
+      <c r="R45" s="2" t="str">
         <f>IF(Projetos!A74&gt;0,Projetos!A74,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="N45" s="3" t="s">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N46" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="O45" s="13" t="s">
+      <c r="O46" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="P46" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="R45" s="2" t="str">
+      <c r="R46" s="2" t="str">
         <f>IF(Projetos!A75&gt;0,Projetos!A75,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="N46" s="3" t="s">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="N47" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="O46" s="13" t="s">
+      <c r="O47" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="P46" s="4" t="s">
+      <c r="P47" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="R46" s="2" t="str">
+      <c r="R47" s="2" t="str">
         <f>IF(Projetos!A76&gt;0,Projetos!A76,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E47" s="42"/>
-      <c r="N47" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="O47" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="P47" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="R47" s="2" t="str">
-        <f>IF(Projetos!A77&gt;0,Projetos!A77,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E48" s="42"/>
       <c r="N48" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R48" s="2" t="str">
-        <f>IF(Projetos!A78&gt;0,Projetos!A78,"")</f>
+        <f>IF(Projetos!A77&gt;0,Projetos!A77,"")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E49" s="42"/>
       <c r="N49" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="P49" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="R49" s="2" t="str">
-        <f>IF(Projetos!A79&gt;0,Projetos!A79,"")</f>
+        <f>IF(Projetos!A78&gt;0,Projetos!A78,"")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E50" s="42"/>
       <c r="N50" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="P50" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="R50" s="2" t="str">
-        <f>IF(Projetos!A80&gt;0,Projetos!A80,"")</f>
+        <f>IF(Projetos!A79&gt;0,Projetos!A79,"")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E51" s="42"/>
       <c r="N51" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="R51" s="2" t="str">
+        <f>IF(Projetos!A80&gt;0,Projetos!A80,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E52" s="42"/>
+      <c r="N52" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="O51" s="3" t="s">
+      <c r="O52" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="P51" s="4" t="s">
+      <c r="P52" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="R51" s="2" t="str">
+      <c r="R52" s="2" t="str">
         <f>IF(Projetos!A81&gt;0,Projetos!A81,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="42"/>
-      <c r="N52" s="3" t="s">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="82"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="42"/>
+      <c r="N53" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="O52" s="3" t="s">
+      <c r="O53" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="P52" s="4" t="s">
+      <c r="P53" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="R52" s="2" t="str">
+      <c r="R53" s="2" t="str">
         <f>IF(Projetos!A82&gt;0,Projetos!A82,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="81"/>
-      <c r="C53" s="81"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="42"/>
-      <c r="N53" s="3" t="s">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="42"/>
+      <c r="N54" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="O53" s="3" t="s">
+      <c r="O54" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="P53" s="4" t="s">
+      <c r="P54" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="R53" s="2" t="str">
+      <c r="R54" s="2" t="str">
         <f>IF(Projetos!A83&gt;0,Projetos!A83,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="82"/>
-      <c r="C54" s="82"/>
-      <c r="D54" s="82"/>
-      <c r="N54" s="3" t="s">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="82"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="82"/>
+      <c r="N55" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="O54" s="3" t="s">
+      <c r="O55" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="P54" s="4" t="s">
+      <c r="P55" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="R54" s="2" t="str">
+      <c r="R55" s="2" t="str">
         <f>IF(Projetos!A84&gt;0,Projetos!A84,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N55" s="3" t="s">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N56" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="O55" s="3" t="s">
+      <c r="O56" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="P55" s="4" t="s">
+      <c r="P56" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="R55" s="2" t="str">
+      <c r="R56" s="2" t="str">
         <f>IF(Projetos!A85&gt;0,Projetos!A85,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N56" s="3" t="s">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N57" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="O56" s="3" t="s">
+      <c r="O57" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="P56" s="4" t="s">
+      <c r="P57" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="R56" s="2" t="str">
+      <c r="R57" s="2" t="str">
         <f>IF(Projetos!A86&gt;0,Projetos!A86,"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N57" s="3" t="s">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N58" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="O57" s="3" t="s">
+      <c r="O58" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="P57" s="4" t="s">
+      <c r="P58" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="R57" s="2" t="str">
+      <c r="R58" s="2" t="str">
         <f>IF(Projetos!A87&gt;0,Projetos!A87,"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N58" s="3" t="s">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N59" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="O58" s="3" t="s">
+      <c r="O59" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="P58" s="4" t="s">
+      <c r="P59" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="R58" s="2" t="str">
+      <c r="R59" s="2" t="str">
         <f>IF(Projetos!A88&gt;0,Projetos!A88,"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N59" s="3" t="s">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N60" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="O59" s="3" t="s">
+      <c r="O60" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="P59" s="4" t="s">
+      <c r="P60" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="R59" s="2" t="str">
+      <c r="R60" s="2" t="str">
         <f>IF(Projetos!A89&gt;0,Projetos!A89,"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N60" s="3" t="s">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N61" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="O60" s="3" t="s">
+      <c r="O61" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="P60" s="4" t="s">
+      <c r="P61" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="R60" s="2" t="str">
+      <c r="R61" s="2" t="str">
         <f>IF(Projetos!A90&gt;0,Projetos!A90,"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N61" s="3" t="s">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N62" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="O61" s="3" t="s">
+      <c r="O62" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="P61" s="4" t="s">
+      <c r="P62" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="R61" s="2" t="str">
+      <c r="R62" s="2" t="str">
         <f>IF(Projetos!A91&gt;0,Projetos!A91,"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N62" s="3" t="s">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N63" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="O62" s="3" t="s">
+      <c r="O63" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="P62" s="4" t="s">
+      <c r="P63" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="R62" s="2" t="str">
+      <c r="R63" s="2" t="str">
         <f>IF(Projetos!A92&gt;0,Projetos!A92,"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N63" s="3" t="s">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N64" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="O63" s="3" t="s">
+      <c r="O64" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="P63" s="4" t="s">
+      <c r="P64" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="R63" s="2" t="str">
+      <c r="R64" s="2" t="str">
         <f>IF(Projetos!A93&gt;0,Projetos!A93,"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N64" s="3" t="s">
+    <row r="65" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N65" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="O64" s="3" t="s">
+      <c r="O65" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="P64" s="4" t="s">
+      <c r="P65" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="R64" s="2" t="str">
+      <c r="R65" s="2" t="str">
         <f>IF(Projetos!A94&gt;0,Projetos!A94,"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="14:18" x14ac:dyDescent="0.2">
-      <c r="N65" s="3" t="s">
+    <row r="66" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N66" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="O65" s="3" t="s">
+      <c r="O66" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="P65" s="4" t="s">
+      <c r="P66" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="R65" s="2" t="str">
+      <c r="R66" s="2" t="str">
         <f>IF(Projetos!A95&gt;0,Projetos!A95,"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="14:18" x14ac:dyDescent="0.2">
-      <c r="N66" s="3" t="s">
+    <row r="67" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N67" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="O66" s="3" t="s">
+      <c r="O67" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P66" s="4" t="s">
+      <c r="P67" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="R66" s="2" t="str">
+      <c r="R67" s="2" t="str">
         <f>IF(Projetos!A96&gt;0,Projetos!A96,"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="14:18" x14ac:dyDescent="0.2">
-      <c r="N67" s="3" t="e">
+    <row r="68" spans="14:18" x14ac:dyDescent="0.2">
+      <c r="N68" s="3" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="O67" s="3" t="e">
+      <c r="O68" s="3" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="P67" s="4">
-        <f>L67* 24</f>
-        <v>0</v>
-      </c>
-      <c r="R67" s="2" t="str">
+      <c r="P68" s="4">
+        <f>L68* 24</f>
+        <v>0</v>
+      </c>
+      <c r="R68" s="2" t="str">
         <f>IF(Projetos!A97&gt;0,Projetos!A97,"")</f>
         <v/>
       </c>
@@ -5572,16 +6067,7 @@
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
-  <mergeCells count="18">
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="F44:L44"/>
-    <mergeCell ref="F9:K9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="A42:E43"/>
-    <mergeCell ref="F42:L43"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="K41:L41"/>
+  <mergeCells count="20">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="F4:L4"/>
     <mergeCell ref="F5:L5"/>
@@ -5591,21 +6077,80 @@
     <mergeCell ref="F7:L7"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="F45:L45"/>
+    <mergeCell ref="F9:K9"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="A43:E44"/>
+    <mergeCell ref="F43:L44"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="C11:K18"/>
+    <mergeCell ref="C36:E36"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="B11:B40 C15:C40">
-    <cfRule type="cellIs" dxfId="6" priority="19" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="B11:B41 C19:C25 C38:C39">
+    <cfRule type="cellIs" dxfId="15" priority="31" stopIfTrue="1" operator="equal">
       <formula>"sábado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="40" operator="equal">
       <formula>"domingo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:D13 C14 D14:D40">
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C11 D19:D25 D38:D39">
+    <cfRule type="cellIs" dxfId="13" priority="19" stopIfTrue="1" operator="equal">
       <formula>"sábado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+      <formula>"domingo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C29 C31:C37">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"sábado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"domingo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:D29 D31:D35 D37">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"sábado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"domingo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"sábado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"domingo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"sábado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"domingo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:C41">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"sábado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"domingo"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D41">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"sábado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"domingo"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>